<commit_message>
sample data and features updated
</commit_message>
<xml_diff>
--- a/features.xlsx
+++ b/features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MTechClasses\Software and Data Engineering\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3549A1-0A22-46B1-91BA-BEAB2BD89285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE240A6-873D-4459-A84C-D654E51DED1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CC3E242-E9CA-487F-A157-20B770264FB4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
   <si>
     <t>Dim.</t>
   </si>
@@ -86,26 +86,10 @@
     <t>FIX</t>
   </si>
   <si>
-    <t>Whether or not the change is a</t>
-  </si>
-  <si>
-    <t>Fixing a defect means that more code is modified or added that</t>
-  </si>
-  <si>
-    <t>defect fix ([17], [30], [32], [67]).</t>
-  </si>
-  <si>
-    <t>need to be tested after the change through running the</t>
-  </si>
-  <si>
     <t>MR</t>
   </si>
   <si>
     <t>If the commit is a merge commit.</t>
-  </si>
-  <si>
-    <t>continuous integration process.
-The number of parents of a commit shows if the commit is a</t>
   </si>
   <si>
     <t>merge commit which required to running the continuous</t>
@@ -379,6 +363,27 @@
   <si>
     <t>the need for running the continuous integration process.
 The type of files changed in the commit indicate the need for the CI process to be run (i.g., changes related to source code files).</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether or not the change is a defect fix </t>
+  </si>
+  <si>
+    <t>Fixing a defect means that more code is modified or added that need to be tested after the change through running the continuous integration process.</t>
+  </si>
+  <si>
+    <t>The number of parents of a commit shows if the commit is a</t>
+  </si>
+  <si>
+    <t>Complex</t>
+  </si>
+  <si>
+    <t>Incorporated</t>
   </si>
 </sst>
 </file>
@@ -426,7 +431,23 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -437,6 +458,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{288EB473-BB23-4EFA-8788-6EA70EF8D0D4}" name="Table1" displayName="Table1" ref="A1:H41" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:H41" xr:uid="{288EB473-BB23-4EFA-8788-6EA70EF8D0D4}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{919288C7-4C74-4898-A34E-FA24BE06C3A5}" name="Dim." dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A7A1B079-2B60-4139-8DC3-39A42E353F2B}" name="Name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{45E9D15A-83EA-44B1-BB27-126BA704F701}" name="Definition (Inspired from)" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{2157E489-6092-4EF5-966F-F4D0AA74B6B9}" name="Rational" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{FEA502EA-0636-40DC-A614-8330A747A342}" name="Direct"/>
+    <tableColumn id="6" xr3:uid="{5DE88312-E9CE-48FF-B01F-D3C627DDF8CB}" name="Calculated"/>
+    <tableColumn id="7" xr3:uid="{D08AD511-23B4-44A4-B06B-616A8A9C80B0}" name="Complex"/>
+    <tableColumn id="8" xr3:uid="{2F6E7DBC-F9B8-4C60-BF4A-30F294E6AB77}" name="Incorporated"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -736,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD02DE0-92B1-4D8C-8D27-54ECABBD492D}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,9 +785,12 @@
     <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="90.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,8 +803,20 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -774,46 +827,46 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -821,49 +874,49 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -871,359 +924,352 @@
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="216" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
+    <row r="22" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="1" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="1" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="2" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1" t="s">
+    </row>
+    <row r="36" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="1" t="s">
+    </row>
+    <row r="37" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="D37" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="1" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>